<commit_message>
finish sankey on funds flow diagram
</commit_message>
<xml_diff>
--- a/data_tidy/2020-12-7-pittman-roberson-fund-flow.xlsx
+++ b/data_tidy/2020-12-7-pittman-roberson-fund-flow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robwiederstein/Dropbox/coding/rproj/hunting_licenses/data_tidy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF91DA0E-2D26-2A4B-91DF-E350F54CE3F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3057E462-EE8C-7B44-9F1C-04A26D342F66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{83DF3D2D-52AB-A24A-974C-70749E3E7405}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29940" windowHeight="18740" xr2:uid="{83DF3D2D-52AB-A24A-974C-70749E3E7405}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>source</t>
   </si>
@@ -66,15 +66,6 @@
     <t>bows-arrows</t>
   </si>
   <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>TX</t>
-  </si>
-  <si>
-    <t>wildlife fund</t>
-  </si>
-  <si>
     <t>hunter ed</t>
   </si>
   <si>
@@ -84,7 +75,10 @@
     <t>wildlife restoration</t>
   </si>
   <si>
-    <t>AK</t>
+    <t>sequestration</t>
+  </si>
+  <si>
+    <t>wildlife</t>
   </si>
 </sst>
 </file>
@@ -436,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3EA804-7D7E-9841-8A6D-CED52430A875}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,7 +458,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>190</v>
@@ -475,7 +469,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>190</v>
@@ -486,7 +480,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>185</v>
@@ -497,7 +491,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>47</v>
@@ -505,46 +499,46 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>11.6</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>599</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
       <c r="C9">
-        <v>474</v>
+        <v>599</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -552,10 +546,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10">
-        <v>120</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -563,109 +557,21 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15">
-        <v>23.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18">
-        <v>23.7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20">
-        <v>0.08</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>